<commit_message>
reading in distillation table
</commit_message>
<xml_diff>
--- a/adios_db/adios_db/test/test_importing/example_data/Average-VLSFO-AMSA-2022.xlsx
+++ b/adios_db/adios_db/test/test_importing/example_data/Average-VLSFO-AMSA-2022.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/chris.barker/Hazmat/GitLab/oil_database/adios_db/adios_db/test/test_importing/example_data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{F7DE523F-8548-DE48-8655-8729A969AD92}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:9_{991AD806-5884-2249-A52E-85708746D840}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="8360" yWindow="1020" windowWidth="23580" windowHeight="17520" xr2:uid="{A4891382-C4C2-C649-BC90-83075B8F427D}"/>
+    <workbookView xWindow="13820" yWindow="500" windowWidth="23580" windowHeight="14400" xr2:uid="{A4891382-C4C2-C649-BC90-83075B8F427D}"/>
   </bookViews>
   <sheets>
     <sheet name="Average-VLSFO-AMSA-2022" sheetId="1" r:id="rId1"/>
@@ -971,8 +971,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D1AE41B5-EBD4-784F-86F2-E9CEA1F05E22}">
   <dimension ref="A1:G86"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="161" zoomScaleNormal="161" workbookViewId="0">
-      <selection activeCell="B1" sqref="B1"/>
+    <sheetView tabSelected="1" topLeftCell="A37" zoomScale="161" zoomScaleNormal="161" workbookViewId="0">
+      <selection activeCell="B51" sqref="B51"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1391,6 +1391,9 @@
       <c r="A48" t="s">
         <v>33</v>
       </c>
+      <c r="B48" t="s">
+        <v>73</v>
+      </c>
     </row>
     <row r="49" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A49" t="s">
@@ -1412,8 +1415,8 @@
       <c r="A51" t="s">
         <v>37</v>
       </c>
-      <c r="B51" t="s">
-        <v>46</v>
+      <c r="B51">
+        <v>100</v>
       </c>
       <c r="C51" t="s">
         <v>74</v>

</xml_diff>

<commit_message>
got SARA reading correctly
</commit_message>
<xml_diff>
--- a/adios_db/adios_db/test/test_importing/example_data/Average-VLSFO-AMSA-2022.xlsx
+++ b/adios_db/adios_db/test/test_importing/example_data/Average-VLSFO-AMSA-2022.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/chris.barker/Hazmat/GitLab/oil_database/adios_db/adios_db/test/test_importing/example_data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:9_{991AD806-5884-2249-A52E-85708746D840}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FF37A6E3-7E96-E546-B519-9A3DB7992837}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="13820" yWindow="500" windowWidth="23580" windowHeight="14400" xr2:uid="{A4891382-C4C2-C649-BC90-83075B8F427D}"/>
+    <workbookView xWindow="12920" yWindow="780" windowWidth="24180" windowHeight="16720" xr2:uid="{A4891382-C4C2-C649-BC90-83075B8F427D}"/>
   </bookViews>
   <sheets>
     <sheet name="Average-VLSFO-AMSA-2022" sheetId="1" r:id="rId1"/>
@@ -520,15 +520,9 @@
     <t>AMSA Average Very Low Sulfer Fuel Oil</t>
   </si>
   <si>
-    <t>AMSA average  LSFO</t>
-  </si>
-  <si>
     <t>Trevor Gilbert, Reef Ecologic, VLSFO Study Report 2022 for Australian Maritime Safety Authority</t>
   </si>
   <si>
-    <t>These are properties of an "average" oi from analysis of 48 oils according to the lRMG380 Specification</t>
-  </si>
-  <si>
     <t>Fresh Oil</t>
   </si>
   <si>
@@ -572,6 +566,12 @@
   </si>
   <si>
     <t>0.12.0</t>
+  </si>
+  <si>
+    <t>AMSA Average  LSFO - RMG380</t>
+  </si>
+  <si>
+    <t>These are properties of an "average" oil from analysis of 48 oils according to the RMG380 Specification</t>
   </si>
 </sst>
 </file>
@@ -971,8 +971,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D1AE41B5-EBD4-784F-86F2-E9CEA1F05E22}">
   <dimension ref="A1:G86"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A37" zoomScale="161" zoomScaleNormal="161" workbookViewId="0">
-      <selection activeCell="B51" sqref="B51"/>
+    <sheetView tabSelected="1" zoomScale="161" zoomScaleNormal="161" workbookViewId="0">
+      <selection activeCell="B10" sqref="B10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -991,7 +991,7 @@
         <v>0</v>
       </c>
       <c r="B1" t="s">
-        <v>181</v>
+        <v>179</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.2">
@@ -1017,7 +1017,7 @@
         <v>8</v>
       </c>
       <c r="B5" t="s">
-        <v>164</v>
+        <v>180</v>
       </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.2">
@@ -1033,7 +1033,7 @@
         <v>2022</v>
       </c>
       <c r="C7" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.2">
@@ -1054,7 +1054,7 @@
         <v>134</v>
       </c>
       <c r="B10">
-        <v>20.420000000000002</v>
+        <v>18.7</v>
       </c>
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.2">
@@ -1084,7 +1084,7 @@
         <v>2</v>
       </c>
       <c r="B13" t="s">
-        <v>166</v>
+        <v>181</v>
       </c>
     </row>
     <row r="15" spans="1:5" x14ac:dyDescent="0.2">
@@ -1097,7 +1097,7 @@
         <v>9</v>
       </c>
       <c r="B16" t="s">
-        <v>167</v>
+        <v>165</v>
       </c>
     </row>
     <row r="17" spans="1:5" x14ac:dyDescent="0.2">
@@ -1105,7 +1105,7 @@
         <v>10</v>
       </c>
       <c r="B17" t="s">
-        <v>168</v>
+        <v>166</v>
       </c>
     </row>
     <row r="18" spans="1:5" x14ac:dyDescent="0.2">
@@ -1118,7 +1118,7 @@
         <v>11</v>
       </c>
       <c r="B19" t="s">
-        <v>169</v>
+        <v>167</v>
       </c>
     </row>
     <row r="20" spans="1:5" x14ac:dyDescent="0.2">
@@ -1190,10 +1190,10 @@
     </row>
     <row r="27" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A27" t="s">
-        <v>170</v>
+        <v>168</v>
       </c>
       <c r="B27" t="s">
-        <v>171</v>
+        <v>169</v>
       </c>
       <c r="C27" t="s">
         <v>62</v>
@@ -1207,13 +1207,13 @@
     </row>
     <row r="28" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A28" t="s">
-        <v>172</v>
+        <v>170</v>
       </c>
       <c r="B28">
         <v>30</v>
       </c>
       <c r="C28" t="s">
-        <v>173</v>
+        <v>171</v>
       </c>
       <c r="D28">
         <v>15</v>
@@ -1224,18 +1224,18 @@
     </row>
     <row r="29" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A29" t="s">
-        <v>174</v>
+        <v>172</v>
       </c>
       <c r="C29" t="s">
-        <v>173</v>
+        <v>171</v>
       </c>
     </row>
     <row r="30" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A30" t="s">
-        <v>180</v>
+        <v>178</v>
       </c>
       <c r="C30" t="s">
-        <v>173</v>
+        <v>171</v>
       </c>
     </row>
     <row r="32" spans="1:5" x14ac:dyDescent="0.2">
@@ -1764,7 +1764,7 @@
         <v>43</v>
       </c>
       <c r="B77" t="s">
-        <v>178</v>
+        <v>176</v>
       </c>
       <c r="C77" t="s">
         <v>46</v>
@@ -1812,7 +1812,7 @@
         <v>49</v>
       </c>
       <c r="B81" t="s">
-        <v>178</v>
+        <v>176</v>
       </c>
       <c r="C81" t="s">
         <v>46</v>
@@ -1832,10 +1832,10 @@
     </row>
     <row r="82" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A82" s="2" t="s">
-        <v>175</v>
+        <v>173</v>
       </c>
       <c r="B82" t="s">
-        <v>176</v>
+        <v>174</v>
       </c>
       <c r="C82">
         <v>0.5</v>
@@ -1852,7 +1852,7 @@
         <v>137</v>
       </c>
       <c r="B83" t="s">
-        <v>177</v>
+        <v>175</v>
       </c>
       <c r="C83">
         <v>10</v>
@@ -1869,7 +1869,7 @@
         <v>138</v>
       </c>
       <c r="B85" t="s">
-        <v>178</v>
+        <v>176</v>
       </c>
       <c r="C85" t="s">
         <v>60</v>
@@ -1886,7 +1886,7 @@
     </row>
     <row r="86" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A86" t="s">
-        <v>179</v>
+        <v>177</v>
       </c>
       <c r="B86" s="2" t="s">
         <v>139</v>

</xml_diff>